<commit_message>
Test Cases file, some minor updates
</commit_message>
<xml_diff>
--- a/data/LoginData.xlsx
+++ b/data/LoginData.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zoran\IdeaProjects\Project\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zoran\IdeaProjects\AutomationExercise\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE94E79-40A3-4149-8FE7-75AACC963E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C4A00F-1BF8-4539-9CC0-AB9F6B407C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="2" r:id="rId1"/>
     <sheet name="AddNew" sheetId="3" r:id="rId2"/>
+    <sheet name="CardData" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
   <si>
     <t>Password</t>
   </si>
@@ -37,9 +38,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>info</t>
-  </si>
-  <si>
     <t>Already registered user, used for valid login test</t>
   </si>
   <si>
@@ -149,6 +147,54 @@
   </si>
   <si>
     <t>Invalid email and password</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Card Number</t>
+  </si>
+  <si>
+    <t>CVV</t>
+  </si>
+  <si>
+    <t>Expiry</t>
+  </si>
+  <si>
+    <t>MasterCard</t>
+  </si>
+  <si>
+    <t>Ryan Mitchell</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>12/30</t>
+  </si>
+  <si>
+    <t>Visa</t>
+  </si>
+  <si>
+    <t>Aaron Diaz</t>
+  </si>
+  <si>
+    <t>JCB</t>
+  </si>
+  <si>
+    <t>Nicholas Martin</t>
+  </si>
+  <si>
+    <t>American Express</t>
+  </si>
+  <si>
+    <t>Ella Davis</t>
+  </si>
+  <si>
+    <t>Charlotte Parker</t>
+  </si>
+  <si>
+    <t>Info</t>
   </si>
 </sst>
 </file>
@@ -177,14 +223,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -194,6 +232,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -219,23 +265,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,8 +567,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78272F59-0BE6-4580-BB6A-E3DB6CBE4E37}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="33.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -532,87 +582,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
+      <c r="D1" s="11" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>3</v>
+      <c r="D2" s="6" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>36</v>
+        <v>6</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -626,120 +676,246 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.21875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.77734375" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.77734375" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.21875" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="5"/>
+    <col min="1" max="1" width="13.21875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.21875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="6" t="s">
+      <c r="D2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" s="6" t="s">
+      <c r="F2" s="8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="8">
+        <v>10000</v>
+      </c>
+      <c r="O2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="N2" s="5">
-        <v>10000</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>32</v>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2119C34-76F1-4DDA-9338-0CC739C25E05}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="12">
+        <v>5304389685336880</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="12">
+        <v>4528050532735230</v>
+      </c>
+      <c r="D3" s="2">
+        <v>680</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="12">
+        <v>3591022531417180</v>
+      </c>
+      <c r="D4" s="2">
+        <v>219</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="12">
+        <v>378756451218358</v>
+      </c>
+      <c r="D5" s="2">
+        <v>3460</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="12">
+        <v>4387673914360650</v>
+      </c>
+      <c r="D6" s="2">
+        <v>106</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>